<commit_message>
Atualização do documento modelo de testes
</commit_message>
<xml_diff>
--- a/Testes/Documentação de Testes - MODELO.xlsx
+++ b/Testes/Documentação de Testes - MODELO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Documentos\Meus Projetos\My Nail Salon\Testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50245DED-EFC2-4BAA-A367-F022D315A063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE346B6C-382D-4722-8101-DABA4ABC295E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{60EB7970-8BE6-4BE5-9238-E82C81D98BC0}"/>
   </bookViews>
@@ -268,6 +268,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -275,9 +278,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -743,7 +743,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -754,28 +754,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
@@ -869,46 +869,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
@@ -917,7 +917,7 @@
       <c r="B8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="12" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -931,7 +931,7 @@
       <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -943,7 +943,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -951,15 +951,15 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="186.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
+    <row r="14" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
       <c r="B14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -979,7 +979,7 @@
       </c>
       <c r="D16"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="203.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Correção documento modelo de testes
</commit_message>
<xml_diff>
--- a/Testes/Documentação de Testes - MODELO.xlsx
+++ b/Testes/Documentação de Testes - MODELO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Documentos\Meus Projetos\My Nail Salon\Testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE346B6C-382D-4722-8101-DABA4ABC295E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425DFCA3-46E6-4A25-9DD7-F524FA5E2F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{60EB7970-8BE6-4BE5-9238-E82C81D98BC0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{60EB7970-8BE6-4BE5-9238-E82C81D98BC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Informações Gerais" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>Ambiente de teste</t>
   </si>
   <si>
-    <t>App/SO</t>
-  </si>
-  <si>
     <t>[Qual navegador?]</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>[Foi necessário incluir algum dado para testar a funcionalidade? Se sim, qual?</t>
+  </si>
+  <si>
+    <t>Navegador</t>
   </si>
 </sst>
 </file>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0A0962-7C6C-4640-A9C3-D61D95AF0094}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -787,18 +787,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -830,15 +830,15 @@
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -854,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3D938E-DFC0-49BD-981D-F091202A4734}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,42 +912,42 @@
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -964,24 +964,24 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16"/>
     </row>
     <row r="17" spans="1:2" ht="203.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2"/>
     </row>

</xml_diff>